<commit_message>
Formatting in Account Sale | Changes in Invoice Generation
</commit_message>
<xml_diff>
--- a/main/catalogue/Producer and Marks.xlsx
+++ b/main/catalogue/Producer and Marks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cypherjac.CYPHERJAC\Desktop\Projects\catalogue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\catalogue\main\catalogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="403">
   <si>
     <t>Bureti Tea Company Ltd</t>
   </si>
@@ -559,12 +559,6 @@
     <t>Tulon</t>
   </si>
   <si>
-    <t>Tea Max</t>
-  </si>
-  <si>
-    <t>Konoito</t>
-  </si>
-  <si>
     <t>Kongoi</t>
   </si>
   <si>
@@ -1225,7 +1219,31 @@
     <t xml:space="preserve">WAREHOUSE </t>
   </si>
   <si>
-    <t>*Kibwari</t>
+    <t>Tea Max Fresh</t>
+  </si>
+  <si>
+    <t>SIGINON WAREHOUSE LIMITED- SHIMANZI</t>
+  </si>
+  <si>
+    <t>SGL001</t>
+  </si>
+  <si>
+    <t>Konoito Tea</t>
+  </si>
+  <si>
+    <t>Kisyet Tea Limited</t>
+  </si>
+  <si>
+    <t>KITL</t>
+  </si>
+  <si>
+    <t>Kisyet Tea</t>
+  </si>
+  <si>
+    <t>UNITED (EA) WAREHOUSES LTD</t>
+  </si>
+  <si>
+    <t>UWL020</t>
   </si>
 </sst>
 </file>
@@ -1676,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G187"/>
+  <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="72" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="58" workbookViewId="0">
+      <selection activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1697,19 +1715,19 @@
         <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1717,13 +1735,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -1733,13 +1751,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -1749,13 +1767,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>96</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
@@ -1765,19 +1783,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>150</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1785,13 +1803,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
@@ -1801,13 +1819,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>151</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
@@ -1817,13 +1835,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>152</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
@@ -1833,13 +1851,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>153</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
@@ -1849,13 +1867,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>102</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
@@ -1865,13 +1883,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>117</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
@@ -1881,13 +1899,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>154</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -1897,13 +1915,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>155</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -1913,13 +1931,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>156</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -1929,13 +1947,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>157</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
@@ -1945,13 +1963,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>158</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -1961,13 +1979,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>98</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
@@ -1977,19 +1995,19 @@
         <v>8</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -1997,19 +2015,19 @@
         <v>8</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>159</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -2017,13 +2035,13 @@
         <v>9</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>160</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
@@ -2033,13 +2051,13 @@
         <v>9</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>161</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
@@ -2049,13 +2067,13 @@
         <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>162</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
@@ -2065,13 +2083,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>163</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
@@ -2081,13 +2099,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>164</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
@@ -2097,13 +2115,13 @@
         <v>11</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>165</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
@@ -2113,13 +2131,13 @@
         <v>11</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>166</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -2129,13 +2147,13 @@
         <v>11</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>167</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
@@ -2145,13 +2163,13 @@
         <v>11</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>168</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
@@ -2161,13 +2179,13 @@
         <v>12</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>100</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
@@ -2177,13 +2195,13 @@
         <v>12</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
@@ -2193,13 +2211,13 @@
         <v>13</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>101</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
@@ -2209,13 +2227,13 @@
         <v>14</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>102</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
@@ -2225,13 +2243,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>103</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
@@ -2241,13 +2259,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>169</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
@@ -2257,13 +2275,13 @@
         <v>15</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>170</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
@@ -2273,13 +2291,13 @@
         <v>15</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>171</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
@@ -2289,13 +2307,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>172</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
@@ -2305,13 +2323,13 @@
         <v>15</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
@@ -2321,13 +2339,13 @@
         <v>16</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
@@ -2337,19 +2355,19 @@
         <v>17</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2357,19 +2375,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>104</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -2383,29 +2401,29 @@
         <v>105</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>173</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -2413,45 +2431,53 @@
         <v>20</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>174</v>
+        <v>394</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
+        <v>272</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>175</v>
+        <v>397</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+        <v>272</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
@@ -2461,13 +2487,13 @@
         <v>21</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
@@ -2477,13 +2503,13 @@
         <v>21</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>106</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
@@ -2493,13 +2519,13 @@
         <v>22</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
@@ -2509,29 +2535,29 @@
         <v>23</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>107</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
@@ -2541,13 +2567,13 @@
         <v>24</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>108</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
@@ -2557,13 +2583,13 @@
         <v>24</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
@@ -2573,13 +2599,13 @@
         <v>25</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>109</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
@@ -2589,13 +2615,13 @@
         <v>26</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>110</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
@@ -2605,13 +2631,13 @@
         <v>26</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
@@ -2621,13 +2647,13 @@
         <v>27</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>111</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
@@ -2637,13 +2663,13 @@
         <v>28</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>112</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
@@ -2653,13 +2679,13 @@
         <v>28</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
@@ -2669,13 +2695,13 @@
         <v>29</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
@@ -2685,13 +2711,13 @@
         <v>29</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
@@ -2701,13 +2727,13 @@
         <v>29</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
@@ -2717,13 +2743,13 @@
         <v>30</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>113</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
@@ -2733,13 +2759,13 @@
         <v>31</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>114</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
@@ -2749,13 +2775,13 @@
         <v>32</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E65" s="18"/>
       <c r="F65" s="18"/>
@@ -2765,13 +2791,13 @@
         <v>33</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
@@ -2781,13 +2807,13 @@
         <v>34</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>116</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
@@ -2798,13 +2824,13 @@
         <v>35</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>117</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
@@ -2814,19 +2840,19 @@
         <v>36</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F69" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -2834,13 +2860,13 @@
         <v>37</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>118</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
@@ -2850,13 +2876,13 @@
         <v>37</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E71" s="18"/>
       <c r="F71" s="18"/>
@@ -2866,13 +2892,13 @@
         <v>37</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
@@ -2882,13 +2908,13 @@
         <v>38</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E73" s="18"/>
       <c r="F73" s="18"/>
@@ -2898,13 +2924,13 @@
         <v>38</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
@@ -2914,19 +2940,19 @@
         <v>39</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>119</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -2934,13 +2960,13 @@
         <v>40</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
@@ -2950,13 +2976,13 @@
         <v>40</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E77" s="18"/>
       <c r="F77" s="18"/>
@@ -2966,13 +2992,13 @@
         <v>41</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>120</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
@@ -2982,13 +3008,13 @@
         <v>42</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E79" s="18"/>
       <c r="F79" s="18"/>
@@ -2998,13 +3024,13 @@
         <v>43</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E80" s="18"/>
       <c r="F80" s="18"/>
@@ -3014,13 +3040,13 @@
         <v>43</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="18"/>
@@ -3030,13 +3056,13 @@
         <v>43</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E82" s="18"/>
       <c r="F82" s="18"/>
@@ -3046,13 +3072,13 @@
         <v>43</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E83" s="18"/>
       <c r="F83" s="18"/>
@@ -3062,13 +3088,13 @@
         <v>43</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E84" s="18"/>
       <c r="F84" s="18"/>
@@ -3078,13 +3104,13 @@
         <v>43</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E85" s="18"/>
       <c r="F85" s="18"/>
@@ -3094,13 +3120,13 @@
         <v>43</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E86" s="18"/>
       <c r="F86" s="18"/>
@@ -3110,13 +3136,13 @@
         <v>43</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E87" s="18"/>
       <c r="F87" s="18"/>
@@ -3126,13 +3152,13 @@
         <v>43</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E88" s="18"/>
       <c r="F88" s="18"/>
@@ -3142,13 +3168,13 @@
         <v>43</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E89" s="18"/>
       <c r="F89" s="18"/>
@@ -3158,13 +3184,13 @@
         <v>43</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
@@ -3174,13 +3200,13 @@
         <v>43</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E91" s="18"/>
       <c r="F91" s="18"/>
@@ -3190,13 +3216,13 @@
         <v>44</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E92" s="18"/>
       <c r="F92" s="18"/>
@@ -3206,13 +3232,13 @@
         <v>44</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E93" s="18"/>
       <c r="F93" s="18"/>
@@ -3222,13 +3248,13 @@
         <v>44</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E94" s="18"/>
       <c r="F94" s="18"/>
@@ -3238,29 +3264,29 @@
         <v>44</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E95" s="18"/>
       <c r="F95" s="18"/>
     </row>
     <row r="96" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D96" s="13" t="s">
         <v>323</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="D96" s="13" t="s">
-        <v>325</v>
       </c>
       <c r="E96" s="18"/>
       <c r="F96" s="18"/>
@@ -3270,13 +3296,13 @@
         <v>45</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C97" s="13" t="s">
         <v>121</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E97" s="18"/>
       <c r="F97" s="18"/>
@@ -3286,13 +3312,13 @@
         <v>46</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E98" s="18"/>
       <c r="F98" s="18"/>
@@ -3302,13 +3328,13 @@
         <v>47</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E99" s="18"/>
       <c r="F99" s="18"/>
@@ -3318,13 +3344,13 @@
         <v>47</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E100" s="18"/>
       <c r="F100" s="18"/>
@@ -3334,13 +3360,13 @@
         <v>47</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E101" s="18"/>
       <c r="F101" s="18"/>
@@ -3350,13 +3376,13 @@
         <v>47</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E102" s="18"/>
       <c r="F102" s="18"/>
@@ -3366,13 +3392,13 @@
         <v>47</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C103" s="13" t="s">
         <v>131</v>
       </c>
       <c r="D103" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E103" s="18"/>
       <c r="F103" s="18"/>
@@ -3382,13 +3408,13 @@
         <v>47</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D104" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E104" s="18"/>
       <c r="F104" s="18"/>
@@ -3398,13 +3424,13 @@
         <v>47</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D105" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E105" s="18"/>
       <c r="F105" s="18"/>
@@ -3414,13 +3440,13 @@
         <v>47</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E106" s="18"/>
       <c r="F106" s="18"/>
@@ -3430,13 +3456,13 @@
         <v>48</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C107" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E107" s="18"/>
       <c r="F107" s="18"/>
@@ -3446,13 +3472,13 @@
         <v>49</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C108" s="13" t="s">
         <v>123</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E108" s="18"/>
       <c r="F108" s="18"/>
@@ -3462,13 +3488,13 @@
         <v>50</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C109" s="13" t="s">
         <v>124</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E109" s="18"/>
       <c r="F109" s="18"/>
@@ -3478,13 +3504,13 @@
         <v>51</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C110" s="13" t="s">
         <v>125</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E110" s="18"/>
       <c r="F110" s="18"/>
@@ -3494,13 +3520,13 @@
         <v>52</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C111" s="13" t="s">
         <v>126</v>
       </c>
       <c r="D111" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E111" s="18"/>
       <c r="F111" s="18"/>
@@ -3510,13 +3536,13 @@
         <v>53</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C112" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D112" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E112" s="18"/>
       <c r="F112" s="18"/>
@@ -3526,13 +3552,13 @@
         <v>53</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D113" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E113" s="18"/>
       <c r="F113" s="18"/>
@@ -3542,13 +3568,13 @@
         <v>54</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C114" s="13" t="s">
         <v>128</v>
       </c>
       <c r="D114" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E114" s="18"/>
       <c r="F114" s="18"/>
@@ -3558,13 +3584,13 @@
         <v>55</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C115" s="13" t="s">
         <v>129</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E115" s="18"/>
       <c r="F115" s="18"/>
@@ -3574,13 +3600,13 @@
         <v>56</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C116" s="13" t="s">
         <v>130</v>
       </c>
       <c r="D116" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E116" s="18"/>
       <c r="F116" s="18"/>
@@ -3590,13 +3616,13 @@
         <v>57</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D117" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E117" s="18"/>
       <c r="F117" s="18"/>
@@ -3606,13 +3632,13 @@
         <v>57</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D118" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E118" s="18"/>
       <c r="F118" s="18"/>
@@ -3622,13 +3648,13 @@
         <v>57</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D119" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E119" s="18"/>
       <c r="F119" s="18"/>
@@ -3638,13 +3664,13 @@
         <v>57</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D120" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E120" s="18"/>
       <c r="F120" s="18"/>
@@ -3654,13 +3680,13 @@
         <v>58</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C121" s="13" t="s">
         <v>132</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E121" s="18"/>
       <c r="F121" s="18"/>
@@ -3670,13 +3696,13 @@
         <v>58</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D122" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E122" s="18"/>
       <c r="F122" s="18"/>
@@ -3686,13 +3712,13 @@
         <v>59</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C123" s="13" t="s">
         <v>133</v>
       </c>
       <c r="D123" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E123" s="18"/>
       <c r="F123" s="18"/>
@@ -3702,13 +3728,13 @@
         <v>60</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D124" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E124" s="18"/>
       <c r="F124" s="18"/>
@@ -3718,13 +3744,13 @@
         <v>60</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D125" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E125" s="18"/>
       <c r="F125" s="18"/>
@@ -3734,13 +3760,13 @@
         <v>60</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D126" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E126" s="18"/>
       <c r="F126" s="18"/>
@@ -3750,13 +3776,13 @@
         <v>61</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D127" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E127" s="18"/>
       <c r="F127" s="18"/>
@@ -3766,13 +3792,13 @@
         <v>61</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D128" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E128" s="18"/>
       <c r="F128" s="18"/>
@@ -3782,13 +3808,13 @@
         <v>62</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D129" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E129" s="18"/>
       <c r="F129" s="18"/>
@@ -3798,13 +3824,13 @@
         <v>62</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D130" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E130" s="18"/>
       <c r="F130" s="18"/>
@@ -3814,13 +3840,13 @@
         <v>62</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E131" s="18"/>
       <c r="F131" s="18"/>
@@ -3830,13 +3856,13 @@
         <v>62</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D132" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E132" s="18"/>
       <c r="F132" s="18"/>
@@ -3846,13 +3872,13 @@
         <v>63</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D133" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E133" s="18"/>
       <c r="F133" s="18"/>
@@ -3862,13 +3888,13 @@
         <v>63</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D134" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E134" s="18"/>
       <c r="F134" s="18"/>
@@ -3878,13 +3904,13 @@
         <v>64</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C135" s="13" t="s">
         <v>134</v>
       </c>
       <c r="D135" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E135" s="18"/>
       <c r="F135" s="18"/>
@@ -3894,13 +3920,13 @@
         <v>65</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C136" s="13" t="s">
         <v>135</v>
       </c>
       <c r="D136" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E136" s="18"/>
       <c r="F136" s="18"/>
@@ -3910,13 +3936,13 @@
         <v>66</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C137" s="13" t="s">
         <v>136</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E137" s="18"/>
       <c r="F137" s="18"/>
@@ -3926,13 +3952,13 @@
         <v>66</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D138" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E138" s="18"/>
       <c r="F138" s="18"/>
@@ -3942,13 +3968,13 @@
         <v>67</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C139" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D139" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E139" s="18"/>
       <c r="F139" s="18"/>
@@ -3958,13 +3984,13 @@
         <v>67</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D140" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E140" s="18"/>
       <c r="F140" s="18"/>
@@ -3974,13 +4000,13 @@
         <v>67</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C141" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D141" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E141" s="18"/>
       <c r="F141" s="18"/>
@@ -3990,13 +4016,13 @@
         <v>68</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C142" s="13" t="s">
         <v>137</v>
       </c>
       <c r="D142" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E142" s="18"/>
       <c r="F142" s="18"/>
@@ -4006,13 +4032,13 @@
         <v>68</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C143" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D143" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E143" s="18"/>
       <c r="F143" s="18"/>
@@ -4022,13 +4048,13 @@
         <v>68</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C144" s="13" t="s">
         <v>136</v>
       </c>
       <c r="D144" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E144" s="18"/>
       <c r="F144" s="18"/>
@@ -4038,13 +4064,13 @@
         <v>68</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D145" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E145" s="18"/>
       <c r="F145" s="18"/>
@@ -4054,13 +4080,13 @@
         <v>68</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C146" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D146" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E146" s="18"/>
       <c r="F146" s="18"/>
@@ -4070,13 +4096,13 @@
         <v>69</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C147" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D147" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E147" s="18"/>
       <c r="F147" s="18"/>
@@ -4086,13 +4112,13 @@
         <v>69</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C148" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D148" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E148" s="18"/>
       <c r="F148" s="18"/>
@@ -4102,13 +4128,13 @@
         <v>69</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C149" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D149" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E149" s="18"/>
       <c r="F149" s="18"/>
@@ -4118,13 +4144,13 @@
         <v>69</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C150" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D150" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E150" s="18"/>
       <c r="F150" s="18"/>
@@ -4134,13 +4160,13 @@
         <v>69</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D151" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E151" s="18"/>
       <c r="F151" s="18"/>
@@ -4150,13 +4176,13 @@
         <v>70</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C152" s="13" t="s">
         <v>138</v>
       </c>
       <c r="D152" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E152" s="18"/>
       <c r="F152" s="18"/>
@@ -4166,13 +4192,13 @@
         <v>71</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C153" s="13" t="s">
         <v>139</v>
       </c>
       <c r="D153" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E153" s="18"/>
       <c r="F153" s="18"/>
@@ -4182,13 +4208,13 @@
         <v>72</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C154" s="13" t="s">
         <v>140</v>
       </c>
       <c r="D154" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E154" s="18"/>
       <c r="F154" s="18"/>
@@ -4198,13 +4224,13 @@
         <v>73</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C155" s="13" t="s">
         <v>141</v>
       </c>
       <c r="D155" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E155" s="18"/>
       <c r="F155" s="18"/>
@@ -4214,13 +4240,13 @@
         <v>73</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C156" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D156" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E156" s="18"/>
       <c r="F156" s="18"/>
@@ -4230,13 +4256,13 @@
         <v>74</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C157" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D157" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E157" s="18"/>
       <c r="F157" s="18"/>
@@ -4246,13 +4272,13 @@
         <v>75</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C158" s="13" t="s">
         <v>142</v>
       </c>
       <c r="D158" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E158" s="18"/>
       <c r="F158" s="18"/>
@@ -4262,13 +4288,13 @@
         <v>76</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C159" s="13" t="s">
         <v>143</v>
       </c>
       <c r="D159" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E159" s="18"/>
       <c r="F159" s="18"/>
@@ -4278,13 +4304,13 @@
         <v>77</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D160" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E160" s="18"/>
       <c r="F160" s="18"/>
@@ -4294,13 +4320,13 @@
         <v>78</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C161" s="13" t="s">
         <v>144</v>
       </c>
       <c r="D161" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E161" s="18"/>
       <c r="F161" s="18"/>
@@ -4310,13 +4336,13 @@
         <v>79</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D162" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E162" s="18"/>
       <c r="F162" s="18"/>
@@ -4326,13 +4352,13 @@
         <v>79</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D163" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E163" s="18"/>
       <c r="F163" s="18"/>
@@ -4342,13 +4368,13 @@
         <v>79</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D164" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E164" s="18"/>
       <c r="F164" s="18"/>
@@ -4358,13 +4384,13 @@
         <v>79</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D165" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E165" s="18"/>
       <c r="F165" s="18"/>
@@ -4374,13 +4400,13 @@
         <v>79</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D166" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E166" s="18"/>
       <c r="F166" s="18"/>
@@ -4390,13 +4416,13 @@
         <v>80</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C167" s="13" t="s">
         <v>145</v>
       </c>
       <c r="D167" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E167" s="18"/>
       <c r="F167" s="18"/>
@@ -4406,13 +4432,13 @@
         <v>81</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D168" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E168" s="18"/>
       <c r="F168" s="18"/>
@@ -4422,13 +4448,13 @@
         <v>81</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D169" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E169" s="18"/>
       <c r="F169" s="18"/>
@@ -4438,13 +4464,13 @@
         <v>81</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D170" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E170" s="18"/>
       <c r="F170" s="18"/>
@@ -4454,13 +4480,13 @@
         <v>82</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C171" s="13" t="s">
         <v>146</v>
       </c>
       <c r="D171" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E171" s="18"/>
       <c r="F171" s="18"/>
@@ -4470,13 +4496,13 @@
         <v>83</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C172" s="13" t="s">
         <v>147</v>
       </c>
       <c r="D172" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E172" s="18"/>
       <c r="F172" s="18"/>
@@ -4486,13 +4512,13 @@
         <v>84</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C173" s="13" t="s">
         <v>148</v>
       </c>
       <c r="D173" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E173" s="18"/>
       <c r="F173" s="18"/>
@@ -4502,13 +4528,13 @@
         <v>85</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D174" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E174" s="18"/>
       <c r="F174" s="18"/>
@@ -4518,13 +4544,13 @@
         <v>86</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D175" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E175" s="18"/>
       <c r="F175" s="18"/>
@@ -4534,13 +4560,13 @@
         <v>87</v>
       </c>
       <c r="B176" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C176" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D176" s="13" t="s">
         <v>372</v>
-      </c>
-      <c r="C176" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D176" s="13" t="s">
-        <v>374</v>
       </c>
       <c r="E176" s="18"/>
       <c r="F176" s="18"/>
@@ -4550,13 +4576,13 @@
         <v>87</v>
       </c>
       <c r="B177" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C177" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D177" s="13" t="s">
         <v>372</v>
-      </c>
-      <c r="C177" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D177" s="13" t="s">
-        <v>374</v>
       </c>
       <c r="E177" s="18"/>
       <c r="F177" s="18"/>
@@ -4566,13 +4592,13 @@
         <v>87</v>
       </c>
       <c r="B178" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C178" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D178" s="13" t="s">
         <v>372</v>
-      </c>
-      <c r="C178" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="D178" s="13" t="s">
-        <v>374</v>
       </c>
       <c r="E178" s="18"/>
       <c r="F178" s="18"/>
@@ -4582,13 +4608,13 @@
         <v>87</v>
       </c>
       <c r="B179" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C179" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D179" s="13" t="s">
         <v>372</v>
-      </c>
-      <c r="C179" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="D179" s="13" t="s">
-        <v>374</v>
       </c>
       <c r="E179" s="18"/>
       <c r="F179" s="18"/>
@@ -4598,13 +4624,13 @@
         <v>87</v>
       </c>
       <c r="B180" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C180" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D180" s="13" t="s">
         <v>372</v>
-      </c>
-      <c r="C180" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="D180" s="13" t="s">
-        <v>374</v>
       </c>
       <c r="E180" s="18"/>
       <c r="F180" s="18"/>
@@ -4614,13 +4640,13 @@
         <v>88</v>
       </c>
       <c r="B181" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="C181" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D181" s="13" t="s">
         <v>375</v>
-      </c>
-      <c r="C181" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="D181" s="13" t="s">
-        <v>377</v>
       </c>
       <c r="E181" s="18"/>
       <c r="F181" s="18"/>
@@ -4630,13 +4656,13 @@
         <v>89</v>
       </c>
       <c r="B182" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C182" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D182" s="13" t="s">
         <v>376</v>
-      </c>
-      <c r="C182" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D182" s="13" t="s">
-        <v>378</v>
       </c>
       <c r="E182" s="18"/>
       <c r="F182" s="18"/>
@@ -4646,13 +4672,13 @@
         <v>89</v>
       </c>
       <c r="B183" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C183" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D183" s="13" t="s">
         <v>376</v>
-      </c>
-      <c r="C183" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D183" s="13" t="s">
-        <v>378</v>
       </c>
       <c r="E183" s="18"/>
       <c r="F183" s="18"/>
@@ -4662,13 +4688,13 @@
         <v>90</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C184" s="13" t="s">
         <v>149</v>
       </c>
       <c r="D184" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E184" s="18"/>
       <c r="F184" s="18"/>
@@ -4678,13 +4704,13 @@
         <v>91</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D185" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E185" s="18"/>
       <c r="F185" s="18"/>
@@ -4694,35 +4720,55 @@
         <v>91</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D186" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E186" s="18"/>
       <c r="F186" s="18"/>
     </row>
-    <row r="187" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C187" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="D187" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E187" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="F187" s="18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C188" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="D188" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E188" s="18" t="s">
         <v>391</v>
       </c>
-      <c r="B187" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C187" s="13" t="s">
+      <c r="F188" s="17" t="s">
         <v>392</v>
-      </c>
-      <c r="D187" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="E187" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="F187" s="17" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -4755,19 +4801,19 @@
         <v>92</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -4775,19 +4821,19 @@
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>150</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -4795,19 +4841,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>99</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -4815,19 +4861,19 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>159</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -4835,19 +4881,19 @@
         <v>17</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -4855,19 +4901,19 @@
         <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>104</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -4875,19 +4921,19 @@
         <v>19</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>173</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4895,19 +4941,19 @@
         <v>36</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -4915,39 +4961,39 @@
         <v>39</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>119</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>105</v>
       </c>
       <c r="E14" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="H14" s="17" t="s">
         <v>392</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>